<commit_message>
I need a better repro
</commit_message>
<xml_diff>
--- a/GeoramaRPG-Project/Assets/_SCR/Data/Source/ItemData.xlsx
+++ b/GeoramaRPG-Project/Assets/_SCR/Data/Source/ItemData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\GitHub\G-RPG\GeoramaRPG-Project\Assets\_SCR\Data\Source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC62A447-D13D-4D60-A395-E771E0F0F0CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D000C7C-AE64-46DB-B03E-D862BB52019D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E36BC707-7DE3-4383-A4FB-ABE29558C2EA}"/>
+    <workbookView xWindow="4170" yWindow="1380" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{E36BC707-7DE3-4383-A4FB-ABE29558C2EA}"/>
   </bookViews>
   <sheets>
     <sheet name="ItemCatalogData" sheetId="1" r:id="rId1"/>
+    <sheet name="InitialInventoryData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -48,6 +49,24 @@
   </si>
   <si>
     <t>GearDB</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>_Notes</t>
+  </si>
+  <si>
+    <t>SetID</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>ItemID</t>
+  </si>
+  <si>
+    <t>Test_1</t>
   </si>
 </sst>
 </file>
@@ -72,15 +91,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -88,13 +113,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C84A7F7-6627-44DB-98E4-3D38D39CDA28}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -440,4 +556,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D807F585-762B-4D8B-BD69-AFF1F2AEE723}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.42578125" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>_xlfn.CONCAT(B2, "_", C2)</f>
+        <v>Default_Test_1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="7"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="11"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>